<commit_message>
enahced scoring criteria, added lookups to determine tier designation, approval level, and required artifact
</commit_message>
<xml_diff>
--- a/Governance.ARB/ARB_Impact_Scoring_template.xlsx
+++ b/Governance.ARB/ARB_Impact_Scoring_template.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitRepository\git\Lab.Architecture\ARB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepository\git\Lab.Architecture\Governance.ARB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F8754C-5A63-440A-A973-73E706FF700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B87F842-866E-4356-8566-4D353FA46DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{F80B5894-3F84-4B3F-8755-7D24C5E9BEEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="499" xr2:uid="{F80B5894-3F84-4B3F-8755-7D24C5E9BEEE}"/>
   </bookViews>
   <sheets>
     <sheet name="ARB Impact Scoring" sheetId="1" r:id="rId1"/>
     <sheet name="Impact Definitions" sheetId="2" r:id="rId2"/>
     <sheet name="Tier Lookup" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Budget_Tier">'Impact Definitions'!$M$2:$M$7</definedName>
+    <definedName name="Business_Impact">'Impact Definitions'!$A$2:$A$7</definedName>
+    <definedName name="Business_Risk_Scope">'Impact Definitions'!$K$2:$K$7</definedName>
+    <definedName name="Highest_Data_Classification">'Impact Definitions'!$C$2:$C$7</definedName>
+    <definedName name="Intereface_Boundary">'Impact Definitions'!$G$2:$G$7</definedName>
+    <definedName name="Interface_Boundary">'Impact Definitions'!$G$2:$G$7</definedName>
+    <definedName name="New_Technology">'Impact Definitions'!$E$2:$E$7</definedName>
+    <definedName name="User_Blast_Radius">'Impact Definitions'!$I$2:$I$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,14 +46,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="64">
   <si>
     <t>Interface Boundary</t>
   </si>
   <si>
-    <t>Business Risk</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -77,12 +84,6 @@
     <t>External - Customers</t>
   </si>
   <si>
-    <t>Visibuility to Users</t>
-  </si>
-  <si>
-    <t>Visibility to Users</t>
-  </si>
-  <si>
     <t>ARB Impact Scoring Dimension</t>
   </si>
   <si>
@@ -98,12 +99,6 @@
     <t>ARB Impact</t>
   </si>
   <si>
-    <t>ARB Impact Score Looup</t>
-  </si>
-  <si>
-    <t>Security Considerations</t>
-  </si>
-  <si>
     <t>PII Data</t>
   </si>
   <si>
@@ -152,17 +147,104 @@
     <t>Tier-1</t>
   </si>
   <si>
-    <t>Tier Designation</t>
-  </si>
-  <si>
     <t>Internal - Corporate</t>
+  </si>
+  <si>
+    <t>ARB Tier Designation</t>
+  </si>
+  <si>
+    <t>Total Impact Score</t>
+  </si>
+  <si>
+    <t>Impact Score</t>
+  </si>
+  <si>
+    <t>Business Impact</t>
+  </si>
+  <si>
+    <t>Highest Data Classification</t>
+  </si>
+  <si>
+    <t>New Technology</t>
+  </si>
+  <si>
+    <t>Desktop</t>
+  </si>
+  <si>
+    <t>Library/Framework</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Multiple/Combination</t>
+  </si>
+  <si>
+    <t>User Blast Radius</t>
+  </si>
+  <si>
+    <t>Business Risk Scope</t>
+  </si>
+  <si>
+    <t>Tier-4</t>
+  </si>
+  <si>
+    <t>ADR</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Tier-5</t>
+  </si>
+  <si>
+    <t>Approval Level</t>
+  </si>
+  <si>
+    <t>Full ARB</t>
+  </si>
+  <si>
+    <t>Partial ARB</t>
+  </si>
+  <si>
+    <t>Assigned EA</t>
+  </si>
+  <si>
+    <t>Solution Architect</t>
+  </si>
+  <si>
+    <t>Change Request</t>
+  </si>
+  <si>
+    <t>Delivery Team</t>
+  </si>
+  <si>
+    <t>SAD - Lightweight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAD  </t>
+  </si>
+  <si>
+    <t>Required Artifact</t>
+  </si>
+  <si>
+    <t>Required Approval Level</t>
+  </si>
+  <si>
+    <t>ARB Impact Score Subtotals</t>
+  </si>
+  <si>
+    <t>Total ARB Impact Score, for Tier Lookup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +260,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,18 +319,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -234,11 +371,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,7 +397,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -255,15 +404,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,49 +545,32 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARB Impact Scoring'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARB Impact Scoring'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Security Considerations</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Interface Boundary</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Visibility to Users</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Business Risk</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Budget Tier</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARB Impact Scoring'!$C$2:$C$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,15 +1321,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2590799</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>2514599</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1203,9 +1358,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1243,7 +1398,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1349,7 +1504,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1491,7 +1646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1499,281 +1654,517 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF2D33A-7BE6-48FE-AEF9-113FEDF0A9CB}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.88671875" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8">
-        <f>VLOOKUP($B2, 'Impact Definitions'!$A$2:$F$6, 6, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="str">
+        <f>'Impact Definitions'!A$1</f>
+        <v>Business Impact</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="15">
+        <f>VLOOKUP($B2, 'Impact Definitions'!$A$2:$B$7, 2, FALSE)</f>
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="8">
-        <f>VLOOKUP($B3, 'Impact Definitions'!$B$2:$F$6, 5, FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="8">
-        <f>VLOOKUP($B4, 'Impact Definitions'!$C$2:$F$6, 4, FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8">
-        <f>VLOOKUP($B5, 'Impact Definitions'!$D$2:$F$6, 3, FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="8">
-        <f>VLOOKUP($B6, 'Impact Definitions'!$E$2:$F$6, 2, FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C7" s="11">
-        <f>SUM(C2:C6)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="10" t="str">
-        <f>VLOOKUP($C$7, 'Tier Lookup'!$A$1:$B$25, 2, FALSE)</f>
-        <v>Tier-1</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="str">
+        <f>'Impact Definitions'!C$1</f>
+        <v>Highest Data Classification</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="15">
+        <f>VLOOKUP($B3, 'Impact Definitions'!$C$2:$D$7, 2, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="str">
+        <f>'Impact Definitions'!E$1</f>
+        <v>New Technology</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="15">
+        <f>VLOOKUP($B4, 'Impact Definitions'!$E$2:$F$7, 2, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="str">
+        <f>'Impact Definitions'!G$1</f>
+        <v>Interface Boundary</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="15">
+        <f>VLOOKUP($B5, 'Impact Definitions'!$G$2:$H$7, 2, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="str">
+        <f>'Impact Definitions'!I$1</f>
+        <v>User Blast Radius</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="15">
+        <f>VLOOKUP($B6, 'Impact Definitions'!$I$2:$J$7, 2, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="str">
+        <f>'Impact Definitions'!K$1</f>
+        <v>Business Risk Scope</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="15">
+        <f>VLOOKUP($B7, 'Impact Definitions'!$K$2:$L$7, 2, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="str">
+        <f>'Impact Definitions'!M$1</f>
+        <v>Budget Tier</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="15">
+        <f>VLOOKUP($B8, 'Impact Definitions'!$M$2:$N$7, 2, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="16">
+        <f>SUM(C2:C8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="str">
+        <f>VLOOKUP($C$9, 'Tier Lookup'!A2:D38, 2, FALSE)</f>
+        <v>No ARB Required</v>
+      </c>
+      <c r="B11" s="20" t="str">
+        <f>VLOOKUP($C$9, 'Tier Lookup'!A2:D38, 3, FALSE)</f>
+        <v>N/A</v>
+      </c>
+      <c r="C11" s="20" t="str">
+        <f>VLOOKUP($C$9, 'Tier Lookup'!A2:D38, 4, FALSE)</f>
+        <v>N/A</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{4D74ED95-317D-4D0E-AF38-8EDBF3C9A8C8}">
+      <formula1>Business_Impact</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{BBDDB236-DEB7-431F-B7DD-2BABF9839637}">
+      <formula1>Highest_Data_Classification</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{F8C6E46E-641C-4FE4-82A9-DBDC7CC693BB}">
+      <formula1>New_Technology</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{6362A96D-2DB8-4D8E-9641-8F75531F3273}">
+      <formula1>Interface_Boundary</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{AE26C2F0-B18C-4242-87CC-93C6AF61D286}">
+      <formula1>User_Blast_Radius</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{85AB26BA-9709-4A6B-8F42-2923A1E8C38F}">
+      <formula1>Business_Risk_Scope</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{8516B455-9A2B-4A2E-A621-C775EC523C0A}">
+      <formula1>Budget_Tier</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7FD26DF3-E473-4E7F-BC3D-C2DF2837ADED}">
-          <x14:formula1>
-            <xm:f>'Impact Definitions'!$A$2:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{021900D9-706A-481E-9320-3896C8BCE246}">
-          <x14:formula1>
-            <xm:f>'Impact Definitions'!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2DB8362D-6FE3-48FC-98C5-E35790C85286}">
-          <x14:formula1>
-            <xm:f>'Impact Definitions'!$C$2:$C$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39239688-A7FD-493D-8638-A24B2285C6A8}">
-          <x14:formula1>
-            <xm:f>'Impact Definitions'!$D$2:$D$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{796BBE72-DE3E-4ED8-870A-CDC0324187BA}">
-          <x14:formula1>
-            <xm:f>'Impact Definitions'!$E$2:$E$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0B844F-60CD-423E-A908-F30824E5B77D}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="47.88671875" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="35.5546875" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="5">
+        <v>2</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="5">
+        <v>2</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="5">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="5">
+        <v>4</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="5">
+        <v>4</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D7" s="5">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="5">
+        <v>5</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="5">
+        <v>5</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="N7" s="5">
         <v>5</v>
       </c>
     </row>
@@ -1785,240 +2176,584 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B082BC0-AE65-406B-A8A3-C53E7A40BA56}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="4" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f>SUM(A2+1)</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f t="shared" ref="A5:A38" si="0">SUM(A4+1)</f>
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <f>SUM(A1+1)</f>
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <f t="shared" ref="A3:A25" si="0">SUM(A2+1)</f>
-        <v>3</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="B37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>37</v>
+      <c r="B38" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>